<commit_message>
DAOS OK && Check Tabela Vazia
</commit_message>
<xml_diff>
--- a/Atividades.xlsx
+++ b/Atividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Ícones dos Botões (3 em cada aba)</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>GRUPO</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +428,7 @@
     <col min="1" max="1" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -447,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -457,8 +460,11 @@
       <c r="H3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -469,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -477,7 +483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -487,8 +493,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -499,7 +508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -510,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>

</xml_diff>